<commit_message>
comparison worst/best correl genes table
</commit_message>
<xml_diff>
--- a/gene_ontology_analysis/GO_results_TAD/TAD_boundries_go_analyzes.xlsx
+++ b/gene_ontology_analysis/GO_results_TAD/TAD_boundries_go_analyzes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10119"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10309"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/beyzakaya/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/beyzakaya/Desktop/timeSeries_HiC/gene_ontology_analysis/GO_results_TAD/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D4B9F14-4F99-1E42-AFAA-F2B4DF7DD69A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E7F3752-E60D-9F43-902C-E278B326F6EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16260" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16260" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Strong_Boundaries_GO_Biologi" sheetId="1" r:id="rId1"/>
@@ -5951,7 +5951,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P30"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="G5" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
@@ -6920,9 +6920,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I672"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="U14" sqref="U14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="6" max="6" width="38" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -26421,8 +26426,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:V76"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+    <sheetView showGridLines="0" topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="S8" sqref="S8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>